<commit_message>
update KPI Library Bp Nofrisel
</commit_message>
<xml_diff>
--- a/1. Dokumen & Literatur/Database Library SO KPI SI versi 5.xlsx
+++ b/1. Dokumen & Literatur/Database Library SO KPI SI versi 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dicha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\1. Dokumen &amp; Literatur\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9338A6E-4FFA-4570-B16D-77036355E252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4AB53D-17F8-465E-8D59-6293FA78D49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -801,6 +801,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1116,10 +1119,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="B1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1127,16 +1131,16 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="20.88671875" style="14" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" customWidth="1"/>
-    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="14" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="39.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="39.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="40.44140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="31.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="35.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="40.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="35.5546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.3">
@@ -1185,100 +1189,94 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>174</v>
+      <c r="B3" s="6"/>
+      <c r="C3" s="13" t="s">
+        <v>176</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E3" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="12">
         <v>3</v>
       </c>
-      <c r="G3" s="12">
-        <v>1</v>
-      </c>
       <c r="H3" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
       <c r="C4" s="13" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E4" s="13">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="G4" s="12">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>140</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I4" s="25"/>
       <c r="J4" s="8" t="s">
-        <v>12</v>
+        <v>159</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+    </row>
+    <row r="5" spans="2:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
       <c r="C5" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E5" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="G5" s="12">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>141</v>
@@ -1287,70 +1285,68 @@
         <v>13</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="M5" s="27"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="6" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
       <c r="C6" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>178</v>
       </c>
       <c r="E6" s="13">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="G6" s="12">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>141</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="I6" s="25"/>
       <c r="J6" s="8" t="s">
-        <v>13</v>
+        <v>159</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="M6" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="N6" s="3"/>
     </row>
     <row r="7" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B7" s="6"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E7" s="13">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G7" s="12">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>141</v>
@@ -1362,82 +1358,82 @@
         <v>14</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>178</v>
       </c>
       <c r="E8" s="13">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="G8" s="12">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
       <c r="C9" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E9" s="13">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="G9" s="12">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" s="24"/>
       <c r="C10" s="23"/>
       <c r="D10" s="23"/>
@@ -1467,42 +1463,40 @@
     <row r="11" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
       <c r="C11" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E11" s="13">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
+    <row r="12" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="2"/>
       <c r="C12" s="13" t="s">
         <v>176</v>
       </c>
@@ -1510,16 +1504,16 @@
         <v>171</v>
       </c>
       <c r="E12" s="13">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G12" s="12">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I12" s="12" t="s">
         <v>141</v>
@@ -1531,30 +1525,34 @@
         <v>15</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="13" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
       <c r="C13" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E13" s="13">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G13" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I13" s="12" t="s">
         <v>141</v>
@@ -1566,30 +1564,32 @@
         <v>14</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="M13" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="N13" s="3"/>
     </row>
     <row r="14" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="13" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E14" s="13">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G14" s="12">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>141</v>
@@ -1601,157 +1601,161 @@
         <v>15</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="M14" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="N14" s="3"/>
     </row>
     <row r="15" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="13" t="s">
-        <v>177</v>
+      <c r="B15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>174</v>
       </c>
       <c r="D15" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E15" s="13">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G15" s="12">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="7"/>
+    </row>
+    <row r="16" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
       <c r="C16" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="E16" s="13">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G16" s="12">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>13</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="I16" s="25"/>
+      <c r="J16" s="26"/>
       <c r="K16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
+    <row r="17" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
       <c r="C17" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E17" s="13">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G17" s="12">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="25"/>
+        <v>62</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="J17" s="8" t="s">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="K17" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B18" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
       <c r="C18" s="13" t="s">
         <v>176</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E18" s="13">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="G18" s="12">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I18" s="25"/>
+        <v>101</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="J18" s="8" t="s">
-        <v>159</v>
+        <v>12</v>
       </c>
       <c r="K18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>82</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B19" s="6"/>
+    <row r="19" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
       <c r="C19" s="13" t="s">
         <v>176</v>
       </c>
@@ -1759,33 +1763,33 @@
         <v>171</v>
       </c>
       <c r="E19" s="13">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="G19" s="12">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J19" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>83</v>
+        <v>119</v>
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15"/>
       <c r="C20" s="17"/>
       <c r="D20" s="16"/>
@@ -1813,24 +1817,24 @@
       <c r="N20" s="3"/>
     </row>
     <row r="21" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E21" s="13">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="G21" s="12">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="I21" s="12" t="s">
         <v>141</v>
@@ -1839,37 +1843,33 @@
         <v>13</v>
       </c>
       <c r="K21" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L21" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>87</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="M21" s="7"/>
+      <c r="N21" s="3"/>
     </row>
     <row r="22" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>178</v>
       </c>
       <c r="E22" s="13">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G22" s="12">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I22" s="12" t="s">
         <v>141</v>
@@ -1881,30 +1881,30 @@
         <v>14</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
     <row r="23" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E23" s="13">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G23" s="12">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I23" s="12" t="s">
         <v>141</v>
@@ -1916,122 +1916,120 @@
         <v>15</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>90</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
     <row r="24" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E24" s="13">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>39</v>
+        <v>116</v>
       </c>
       <c r="G24" s="12">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="I24" s="25"/>
-      <c r="J24" s="26"/>
+        <v>117</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="K24" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>92</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
     <row r="25" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E25" s="13">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="G25" s="12">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>62</v>
+        <v>133</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K25" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>95</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
     </row>
     <row r="26" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E26" s="13">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="G26" s="12">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="I26" s="12" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="J26" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="M26" s="3"/>
+        <v>144</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>145</v>
+      </c>
       <c r="N26" s="3"/>
     </row>
     <row r="27" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="13" t="s">
         <v>175</v>
       </c>
@@ -2039,16 +2037,16 @@
         <v>180</v>
       </c>
       <c r="E27" s="13">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="G27" s="12">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="I27" s="12" t="s">
         <v>140</v>
@@ -2057,37 +2055,35 @@
         <v>12</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>99</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N27" s="7"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E28" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="G28" s="12">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>140</v>
@@ -2099,33 +2095,37 @@
         <v>14</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="M28" s="3"/>
-      <c r="N28" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="29" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="13" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E29" s="13">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="G29" s="12">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>103</v>
+        <v>147</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="J29" s="8" t="s">
         <v>12</v>
@@ -2134,7 +2134,7 @@
         <v>14</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>119</v>
+        <v>148</v>
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
@@ -2142,76 +2142,76 @@
     <row r="30" spans="2:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E30" s="13">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="G30" s="12">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="H30" s="8" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="I30" s="12" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="M30" s="3" t="s">
-        <v>121</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E31" s="13">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="G31" s="12">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H31" s="8" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K31" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="M31" s="3"/>
+        <v>154</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" s="19"/>
       <c r="C32" s="17"/>
       <c r="D32" s="16"/>
@@ -2236,7 +2236,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B33" s="19"/>
       <c r="C33" s="17"/>
       <c r="D33" s="16"/>
@@ -2263,7 +2263,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="2:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="13" t="s">
         <v>177</v>
@@ -2300,7 +2300,7 @@
       </c>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" s="19"/>
       <c r="C35" s="17"/>
       <c r="D35" s="16"/>
@@ -2330,61 +2330,57 @@
     <row r="36" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="13" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E36" s="13">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F36" s="8" t="s">
-        <v>112</v>
+        <v>156</v>
       </c>
       <c r="G36" s="12">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H36" s="8" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="I36" s="12" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="J36" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K36" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L36" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="M36" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="N36" s="3" t="s">
-        <v>128</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
     </row>
     <row r="37" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B37" s="2"/>
+      <c r="B37" s="6"/>
       <c r="C37" s="13" t="s">
         <v>177</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E37" s="13">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>114</v>
+        <v>24</v>
       </c>
       <c r="G37" s="12">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="I37" s="12" t="s">
         <v>141</v>
@@ -2396,67 +2392,65 @@
         <v>14</v>
       </c>
       <c r="L37" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>130</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B38" s="2"/>
+      <c r="B38" s="6"/>
       <c r="C38" s="13" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>178</v>
       </c>
       <c r="E38" s="13">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="G38" s="12">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="I38" s="12" t="s">
-        <v>166</v>
+        <v>141</v>
       </c>
       <c r="J38" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K38" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L38" s="8" t="s">
-        <v>131</v>
+        <v>67</v>
       </c>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="2"/>
+      <c r="B39" s="6"/>
       <c r="C39" s="13" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E39" s="13">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>132</v>
+        <v>27</v>
       </c>
       <c r="G39" s="12">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>133</v>
+        <v>48</v>
       </c>
       <c r="I39" s="12" t="s">
         <v>141</v>
@@ -2468,12 +2462,14 @@
         <v>14</v>
       </c>
       <c r="L39" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="M39" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" s="19"/>
       <c r="C40" s="17"/>
       <c r="D40" s="16"/>
@@ -2501,24 +2497,24 @@
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B41" s="2"/>
+      <c r="B41" s="6"/>
       <c r="C41" s="13" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E41" s="13">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>136</v>
+        <v>31</v>
       </c>
       <c r="G41" s="12">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="H41" s="8" t="s">
-        <v>137</v>
+        <v>52</v>
       </c>
       <c r="I41" s="12" t="s">
         <v>140</v>
@@ -2527,82 +2523,86 @@
         <v>12</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L41" s="8" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="N41" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="42" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E42" s="13">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="G42" s="12">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="H42" s="8" t="s">
-        <v>147</v>
+        <v>106</v>
       </c>
       <c r="I42" s="12" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="J42" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K42" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L42" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="M42" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="N42" s="3"/>
     </row>
     <row r="43" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>180</v>
       </c>
       <c r="E43" s="13">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
       <c r="G43" s="12">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="H43" s="8" t="s">
-        <v>150</v>
+        <v>107</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="J43" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K43" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L43" s="8" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -2610,73 +2610,77 @@
     <row r="44" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E44" s="13">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="G44" s="12">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H44" s="8" t="s">
-        <v>153</v>
+        <v>113</v>
       </c>
       <c r="I44" s="12" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="J44" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K44" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L44" s="8" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="N44" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="N44" s="3" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="45" spans="2:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="13" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E45" s="13">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>156</v>
+        <v>114</v>
       </c>
       <c r="G45" s="12">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H45" s="8" t="s">
-        <v>157</v>
+        <v>115</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>167</v>
+        <v>141</v>
       </c>
       <c r="J45" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="K45" s="8" t="s">
         <v>14</v>
       </c>
       <c r="L45" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="M45" s="3"/>
+        <v>129</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="N45" s="3"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.3">
@@ -2995,7 +2999,17 @@
       <c r="N66" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:N45" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}"/>
+  <autoFilter ref="B2:N45" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Kualitas"/>
+        <filter val="Produktivitas"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N45">
+      <sortCondition ref="C2:C45"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>